<commit_message>
load observation using drift
</commit_message>
<xml_diff>
--- a/lib/admin/observationList.xlsx
+++ b/lib/admin/observationList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majona\GitHub\flutter_application_1\lib\admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majona\GitHub\iko_reliability_flutter\lib\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D83B5D-0527-4A3F-8FDE-0E98C3FD3BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC1EC7D-C45F-40AC-AADB-572F078808BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09758C92-894A-4C5A-8743-6DDC127AC6B4}"/>
   </bookViews>
@@ -26932,7 +26932,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -27001,7 +27001,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -27330,8 +27330,8 @@
   </sheetPr>
   <dimension ref="A1:P3145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E349" sqref="E349"/>
+    <sheetView tabSelected="1" topLeftCell="A3074" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3094" sqref="I3094"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76700,7 +76700,7 @@
     </row>
     <row r="3080" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F3080" s="2" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="G3080" s="2" t="s">
         <v>2102</v>

</xml_diff>